<commit_message>
multiChecking done, time to other minerals testing and similarity refined
</commit_message>
<xml_diff>
--- a/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
+++ b/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
@@ -19,7 +19,6 @@
     <sheet name="Hausdorff" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1137,11 +1136,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360590056"/>
-        <c:axId val="360590840"/>
+        <c:axId val="355048808"/>
+        <c:axId val="355052336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360590056"/>
+        <c:axId val="355048808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,12 +1197,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360590840"/>
+        <c:crossAx val="355052336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360590840"/>
+        <c:axId val="355052336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,7 +1259,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360590056"/>
+        <c:crossAx val="355048808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1324,7 +1323,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1410,7 +1408,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1505,11 +1502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360564968"/>
-        <c:axId val="360569672"/>
+        <c:axId val="430855976"/>
+        <c:axId val="430854016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360564968"/>
+        <c:axId val="430855976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,12 +1563,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360569672"/>
+        <c:crossAx val="430854016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360569672"/>
+        <c:axId val="430854016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,7 +1625,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360564968"/>
+        <c:crossAx val="430855976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1692,7 +1689,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1778,7 +1774,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1873,11 +1868,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360568888"/>
-        <c:axId val="360572024"/>
+        <c:axId val="430852840"/>
+        <c:axId val="431497832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360568888"/>
+        <c:axId val="430852840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,12 +1929,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360572024"/>
+        <c:crossAx val="431497832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360572024"/>
+        <c:axId val="431497832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +1991,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360568888"/>
+        <c:crossAx val="430852840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2085,7 +2080,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2171,7 +2165,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2266,11 +2259,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360572416"/>
-        <c:axId val="360564184"/>
+        <c:axId val="431502536"/>
+        <c:axId val="431504888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360572416"/>
+        <c:axId val="431502536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2327,12 +2320,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360564184"/>
+        <c:crossAx val="431504888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360564184"/>
+        <c:axId val="431504888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,7 +2382,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360572416"/>
+        <c:crossAx val="431502536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2486,7 +2479,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2622,11 +2614,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360573592"/>
-        <c:axId val="360573984"/>
+        <c:axId val="431504496"/>
+        <c:axId val="431505280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360573592"/>
+        <c:axId val="431504496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2683,12 +2675,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360573984"/>
+        <c:crossAx val="431505280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360573984"/>
+        <c:axId val="431505280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2745,7 +2737,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360573592"/>
+        <c:crossAx val="431504496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2842,7 +2834,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2928,7 +2919,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3023,11 +3013,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360575160"/>
-        <c:axId val="360563400"/>
+        <c:axId val="431499008"/>
+        <c:axId val="431499400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360575160"/>
+        <c:axId val="431499008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3084,12 +3074,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360563400"/>
+        <c:crossAx val="431499400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360563400"/>
+        <c:axId val="431499400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3146,7 +3136,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360575160"/>
+        <c:crossAx val="431499008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3235,7 +3225,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3321,7 +3310,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3416,11 +3404,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360565752"/>
-        <c:axId val="360566144"/>
+        <c:axId val="431504104"/>
+        <c:axId val="431498616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360565752"/>
+        <c:axId val="431504104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3477,12 +3465,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360566144"/>
+        <c:crossAx val="431498616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360566144"/>
+        <c:axId val="431498616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3539,7 +3527,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360565752"/>
+        <c:crossAx val="431504104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3628,7 +3616,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3764,11 +3751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360567712"/>
-        <c:axId val="360568496"/>
+        <c:axId val="431501752"/>
+        <c:axId val="431503320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360567712"/>
+        <c:axId val="431501752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3825,12 +3812,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360568496"/>
+        <c:crossAx val="431503320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360568496"/>
+        <c:axId val="431503320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3887,7 +3874,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360567712"/>
+        <c:crossAx val="431501752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3976,7 +3963,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4062,7 +4048,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4157,11 +4142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360586136"/>
-        <c:axId val="360580648"/>
+        <c:axId val="431500184"/>
+        <c:axId val="431500576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360586136"/>
+        <c:axId val="431500184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4218,12 +4203,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360580648"/>
+        <c:crossAx val="431500576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360580648"/>
+        <c:axId val="431500576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4280,7 +4265,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360586136"/>
+        <c:crossAx val="431500184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4369,7 +4354,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4642,9 +4626,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4767,9 +4749,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4873,11 +4853,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360582216"/>
-        <c:axId val="360583000"/>
+        <c:axId val="432742272"/>
+        <c:axId val="432741488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360582216"/>
+        <c:axId val="432742272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4934,12 +4914,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360583000"/>
+        <c:crossAx val="432741488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360583000"/>
+        <c:axId val="432741488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4996,7 +4976,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360582216"/>
+        <c:crossAx val="432742272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5086,7 +5066,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5222,11 +5201,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360578296"/>
-        <c:axId val="360586920"/>
+        <c:axId val="432741096"/>
+        <c:axId val="432741880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360578296"/>
+        <c:axId val="432741096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5283,12 +5262,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360586920"/>
+        <c:crossAx val="432741880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360586920"/>
+        <c:axId val="432741880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5345,7 +5324,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360578296"/>
+        <c:crossAx val="432741096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5590,11 +5569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360591232"/>
-        <c:axId val="360594760"/>
+        <c:axId val="355050376"/>
+        <c:axId val="355052728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360591232"/>
+        <c:axId val="355050376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5651,12 +5630,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360594760"/>
+        <c:crossAx val="355052728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360594760"/>
+        <c:axId val="355052728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5713,7 +5692,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360591232"/>
+        <c:crossAx val="355050376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5802,7 +5781,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5988,11 +5966,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360579472"/>
-        <c:axId val="360585352"/>
+        <c:axId val="432743056"/>
+        <c:axId val="432743840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360579472"/>
+        <c:axId val="432743056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6049,12 +6027,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360585352"/>
+        <c:crossAx val="432743840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360585352"/>
+        <c:axId val="432743840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6111,7 +6089,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360579472"/>
+        <c:crossAx val="432743056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6200,7 +6178,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6386,11 +6363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499989192"/>
-        <c:axId val="499988800"/>
+        <c:axId val="432736392"/>
+        <c:axId val="432734824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499989192"/>
+        <c:axId val="432736392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6447,12 +6424,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499988800"/>
+        <c:crossAx val="432734824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499988800"/>
+        <c:axId val="432734824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6509,7 +6486,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499989192"/>
+        <c:crossAx val="432736392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6754,11 +6731,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360592016"/>
-        <c:axId val="360588096"/>
+        <c:axId val="355053904"/>
+        <c:axId val="355054296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360592016"/>
+        <c:axId val="355053904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6815,12 +6792,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360588096"/>
+        <c:crossAx val="355054296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360588096"/>
+        <c:axId val="355054296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6877,7 +6854,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360592016"/>
+        <c:crossAx val="355053904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7122,11 +7099,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360592408"/>
-        <c:axId val="360592800"/>
+        <c:axId val="355056256"/>
+        <c:axId val="355049200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360592408"/>
+        <c:axId val="355056256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7183,12 +7160,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360592800"/>
+        <c:crossAx val="355049200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360592800"/>
+        <c:axId val="355049200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7245,7 +7222,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360592408"/>
+        <c:crossAx val="355056256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7445,11 +7422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360589272"/>
-        <c:axId val="360591624"/>
+        <c:axId val="430849704"/>
+        <c:axId val="430855192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360589272"/>
+        <c:axId val="430849704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7506,12 +7483,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360591624"/>
+        <c:crossAx val="430855192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360591624"/>
+        <c:axId val="430855192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7568,7 +7545,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360589272"/>
+        <c:crossAx val="430849704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7813,11 +7790,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360593192"/>
-        <c:axId val="360570064"/>
+        <c:axId val="430850096"/>
+        <c:axId val="430856368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360593192"/>
+        <c:axId val="430850096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7874,12 +7851,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360570064"/>
+        <c:crossAx val="430856368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360570064"/>
+        <c:axId val="430856368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7936,7 +7913,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360593192"/>
+        <c:crossAx val="430850096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8000,7 +7977,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8086,7 +8062,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8181,11 +8156,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360572808"/>
-        <c:axId val="360566536"/>
+        <c:axId val="430848920"/>
+        <c:axId val="430853232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360572808"/>
+        <c:axId val="430848920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8242,12 +8217,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360566536"/>
+        <c:crossAx val="430853232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360566536"/>
+        <c:axId val="430853232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8304,7 +8279,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360572808"/>
+        <c:crossAx val="430848920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8368,7 +8343,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8454,7 +8428,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8549,11 +8522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360574768"/>
-        <c:axId val="360564576"/>
+        <c:axId val="430850488"/>
+        <c:axId val="430850880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360574768"/>
+        <c:axId val="430850488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8610,12 +8583,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360564576"/>
+        <c:crossAx val="430850880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360564576"/>
+        <c:axId val="430850880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8672,7 +8645,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360574768"/>
+        <c:crossAx val="430850488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8736,7 +8709,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8822,7 +8794,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8917,11 +8888,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360570848"/>
-        <c:axId val="360570456"/>
+        <c:axId val="430851272"/>
+        <c:axId val="430852056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360570848"/>
+        <c:axId val="430851272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8978,12 +8949,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360570456"/>
+        <c:crossAx val="430852056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360570456"/>
+        <c:axId val="430852056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9040,7 +9011,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360570848"/>
+        <c:crossAx val="430851272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21732,8 +21703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -22145,6 +22116,24 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C12" s="5">
+        <v>7.2392999999999999E-2</v>
+      </c>
+      <c r="D12" s="5">
+        <v>6.4041000000000001E-2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>4.3598999999999999E-2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>3.5527999999999997E-2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5.2534999999999998E-2</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2.7650000000000001E-2</v>
+      </c>
       <c r="M12">
         <v>6.4041000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
DT video meeting PPT done, time to solve 2Q in PPT
</commit_message>
<xml_diff>
--- a/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
+++ b/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PosGeneral_SimGau" sheetId="1" r:id="rId1"/>
@@ -1145,11 +1145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="357262664"/>
-        <c:axId val="358292600"/>
+        <c:axId val="101417208"/>
+        <c:axId val="101413288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="357262664"/>
+        <c:axId val="101417208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,12 +1206,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358292600"/>
+        <c:crossAx val="101413288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358292600"/>
+        <c:axId val="101413288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1268,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357262664"/>
+        <c:crossAx val="101417208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1513,11 +1513,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427066840"/>
-        <c:axId val="427068800"/>
+        <c:axId val="239170656"/>
+        <c:axId val="239174576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427066840"/>
+        <c:axId val="239170656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,12 +1574,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427068800"/>
+        <c:crossAx val="239174576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427068800"/>
+        <c:axId val="239174576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1636,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427066840"/>
+        <c:crossAx val="239170656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1700,6 +1700,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1785,6 +1786,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1879,11 +1881,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427065272"/>
-        <c:axId val="427069584"/>
+        <c:axId val="239174184"/>
+        <c:axId val="239171440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427065272"/>
+        <c:axId val="239174184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,12 +1942,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427069584"/>
+        <c:crossAx val="239171440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427069584"/>
+        <c:axId val="239171440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,7 +2004,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427065272"/>
+        <c:crossAx val="239174184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2066,6 +2068,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2151,6 +2154,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2245,11 +2249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427066448"/>
-        <c:axId val="427070368"/>
+        <c:axId val="239169480"/>
+        <c:axId val="239169088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427066448"/>
+        <c:axId val="239169480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,12 +2310,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427070368"/>
+        <c:crossAx val="239169088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427070368"/>
+        <c:axId val="239169088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +2372,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427066448"/>
+        <c:crossAx val="239169480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2457,6 +2461,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2542,6 +2547,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2636,11 +2642,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427071936"/>
-        <c:axId val="427065664"/>
+        <c:axId val="239174968"/>
+        <c:axId val="239172224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427071936"/>
+        <c:axId val="239174968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,12 +2703,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427065664"/>
+        <c:crossAx val="239172224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427065664"/>
+        <c:axId val="239172224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2759,7 +2765,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427071936"/>
+        <c:crossAx val="239174968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2856,6 +2862,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2991,11 +2998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358289072"/>
-        <c:axId val="358287112"/>
+        <c:axId val="239173008"/>
+        <c:axId val="240602472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358289072"/>
+        <c:axId val="239173008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3052,12 +3059,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358287112"/>
+        <c:crossAx val="240602472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358287112"/>
+        <c:axId val="240602472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3114,7 +3121,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358289072"/>
+        <c:crossAx val="239173008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3211,6 +3218,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3296,6 +3304,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3390,11 +3399,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358287504"/>
-        <c:axId val="358287896"/>
+        <c:axId val="240603648"/>
+        <c:axId val="240607960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358287504"/>
+        <c:axId val="240603648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3451,12 +3460,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358287896"/>
+        <c:crossAx val="240607960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358287896"/>
+        <c:axId val="240607960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3513,7 +3522,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358287504"/>
+        <c:crossAx val="240603648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3602,6 +3611,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3687,6 +3697,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3781,11 +3792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358108864"/>
-        <c:axId val="358102984"/>
+        <c:axId val="240604824"/>
+        <c:axId val="240607176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358108864"/>
+        <c:axId val="240604824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3842,12 +3853,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358102984"/>
+        <c:crossAx val="240607176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358102984"/>
+        <c:axId val="240607176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3904,7 +3915,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358108864"/>
+        <c:crossAx val="240604824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3993,6 +4004,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4128,11 +4140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358102200"/>
-        <c:axId val="358103376"/>
+        <c:axId val="240605216"/>
+        <c:axId val="240604040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358102200"/>
+        <c:axId val="240605216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4189,12 +4201,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358103376"/>
+        <c:crossAx val="240604040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358103376"/>
+        <c:axId val="240604040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4251,7 +4263,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358102200"/>
+        <c:crossAx val="240605216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4340,6 +4352,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4425,6 +4438,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4519,11 +4533,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358104160"/>
-        <c:axId val="358104552"/>
+        <c:axId val="240605608"/>
+        <c:axId val="240606000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358104160"/>
+        <c:axId val="240605608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4580,12 +4594,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358104552"/>
+        <c:crossAx val="240606000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358104552"/>
+        <c:axId val="240606000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4642,7 +4656,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358104160"/>
+        <c:crossAx val="240605608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4731,6 +4745,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5003,7 +5018,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5126,7 +5143,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5230,11 +5249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358106120"/>
-        <c:axId val="358106904"/>
+        <c:axId val="240600512"/>
+        <c:axId val="240603256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358106120"/>
+        <c:axId val="240600512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5291,12 +5310,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358106904"/>
+        <c:crossAx val="240603256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358106904"/>
+        <c:axId val="240603256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5353,7 +5372,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358106120"/>
+        <c:crossAx val="240600512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5418,6 +5437,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5503,6 +5523,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5597,11 +5618,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358293384"/>
-        <c:axId val="358293776"/>
+        <c:axId val="101417600"/>
+        <c:axId val="101414856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358293384"/>
+        <c:axId val="101417600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5658,12 +5679,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358293776"/>
+        <c:crossAx val="101414856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358293776"/>
+        <c:axId val="101414856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5720,7 +5741,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358293384"/>
+        <c:crossAx val="101417600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5809,6 +5830,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5944,11 +5966,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358107296"/>
-        <c:axId val="358105336"/>
+        <c:axId val="240601296"/>
+        <c:axId val="240601688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358107296"/>
+        <c:axId val="240601296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6005,12 +6027,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358105336"/>
+        <c:crossAx val="240601688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358105336"/>
+        <c:axId val="240601688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6067,7 +6089,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358107296"/>
+        <c:crossAx val="240601296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6156,6 +6178,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6341,11 +6364,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358107688"/>
-        <c:axId val="358109256"/>
+        <c:axId val="241096376"/>
+        <c:axId val="241099512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358107688"/>
+        <c:axId val="241096376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6402,12 +6425,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358109256"/>
+        <c:crossAx val="241099512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358109256"/>
+        <c:axId val="241099512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6464,7 +6487,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358107688"/>
+        <c:crossAx val="241096376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6553,6 +6576,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6738,11 +6762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358102592"/>
-        <c:axId val="428143912"/>
+        <c:axId val="241097552"/>
+        <c:axId val="241090888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358102592"/>
+        <c:axId val="241097552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6799,12 +6823,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="428143912"/>
+        <c:crossAx val="241090888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="428143912"/>
+        <c:axId val="241090888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6861,7 +6885,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358102592"/>
+        <c:crossAx val="241097552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7106,11 +7130,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358292992"/>
-        <c:axId val="358294168"/>
+        <c:axId val="101413680"/>
+        <c:axId val="101414072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358292992"/>
+        <c:axId val="101413680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7167,12 +7191,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358294168"/>
+        <c:crossAx val="101414072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358294168"/>
+        <c:axId val="101414072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7229,7 +7253,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358292992"/>
+        <c:crossAx val="101413680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7293,6 +7317,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7378,6 +7403,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -7472,11 +7498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358294560"/>
-        <c:axId val="358291032"/>
+        <c:axId val="101412504"/>
+        <c:axId val="101418384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358294560"/>
+        <c:axId val="101412504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7533,12 +7559,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358291032"/>
+        <c:crossAx val="101418384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358291032"/>
+        <c:axId val="101418384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7595,7 +7621,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358294560"/>
+        <c:crossAx val="101412504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7794,11 +7820,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358288680"/>
-        <c:axId val="358288288"/>
+        <c:axId val="101412896"/>
+        <c:axId val="101415640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358288680"/>
+        <c:axId val="101412896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7855,12 +7881,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358288288"/>
+        <c:crossAx val="101415640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358288288"/>
+        <c:axId val="101415640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7917,7 +7943,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358288680"/>
+        <c:crossAx val="101412896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8160,11 +8186,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358289856"/>
-        <c:axId val="427067232"/>
+        <c:axId val="101414464"/>
+        <c:axId val="101419168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358289856"/>
+        <c:axId val="101414464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8221,12 +8247,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427067232"/>
+        <c:crossAx val="101419168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427067232"/>
+        <c:axId val="101419168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8283,7 +8309,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358289856"/>
+        <c:crossAx val="101414464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8528,11 +8554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="433180632"/>
-        <c:axId val="433178672"/>
+        <c:axId val="101419560"/>
+        <c:axId val="101415248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="433180632"/>
+        <c:axId val="101419560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8589,12 +8615,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433178672"/>
+        <c:crossAx val="101415248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="433178672"/>
+        <c:axId val="101415248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8651,7 +8677,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433180632"/>
+        <c:crossAx val="101419560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8896,11 +8922,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427064880"/>
-        <c:axId val="427068408"/>
+        <c:axId val="239170264"/>
+        <c:axId val="239171048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427064880"/>
+        <c:axId val="239170264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8957,12 +8983,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427068408"/>
+        <c:crossAx val="239171048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427068408"/>
+        <c:axId val="239171048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9019,7 +9045,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427064880"/>
+        <c:crossAx val="239170264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9264,11 +9290,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="427069192"/>
-        <c:axId val="427071544"/>
+        <c:axId val="239175360"/>
+        <c:axId val="239169872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="427069192"/>
+        <c:axId val="239175360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9325,12 +9351,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427071544"/>
+        <c:crossAx val="239169872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="427071544"/>
+        <c:axId val="239169872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9387,7 +9413,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427069192"/>
+        <c:crossAx val="239175360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21858,15 +21884,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22671,7 +22697,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23499,8 +23525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23732,7 +23758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
@@ -24052,8 +24078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="A1:J8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -24329,8 +24355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J8"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -24603,8 +24629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
docs almost done, time to run DT custom lib of multiple minerals
</commit_message>
<xml_diff>
--- a/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
+++ b/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PosGeneral_SimGau" sheetId="1" r:id="rId1"/>
     <sheet name="Band2-90%" sheetId="6" r:id="rId2"/>
     <sheet name="PosGeneral_SimCorrcoef" sheetId="2" r:id="rId3"/>
     <sheet name="Possibility" sheetId="3" r:id="rId4"/>
-    <sheet name="PosGen_SimFrechet" sheetId="4" r:id="rId5"/>
-    <sheet name="Hausdorff" sheetId="5" r:id="rId6"/>
+    <sheet name="WeightTesting" sheetId="7" r:id="rId5"/>
+    <sheet name="PosGen_SimFrechet" sheetId="4" r:id="rId6"/>
+    <sheet name="Hausdorff" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
   <si>
     <t>Original Matching</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -270,6 +271,46 @@
     <t>Summation</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>band1(705- 769)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight of center</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-squared</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proxy-value-sub1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub3</t>
+  </si>
+  <si>
+    <t>Sub4</t>
+  </si>
+  <si>
+    <t>Sub5</t>
+  </si>
+  <si>
+    <t>Sub6</t>
+  </si>
+  <si>
+    <t>band2(770-832)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>band3(854-879)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -278,7 +319,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +480,14 @@
       <sz val="10"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="39">
@@ -828,7 +877,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -882,6 +931,12 @@
     </xf>
     <xf numFmtId="176" fontId="3" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -964,7 +1019,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1050,7 +1104,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1145,11 +1198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101417208"/>
-        <c:axId val="101413288"/>
+        <c:axId val="474867016"/>
+        <c:axId val="474864664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101417208"/>
+        <c:axId val="474867016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,12 +1259,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101413288"/>
+        <c:crossAx val="474864664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101413288"/>
+        <c:axId val="474864664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1321,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101417208"/>
+        <c:crossAx val="474867016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1332,7 +1385,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1418,7 +1470,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1513,11 +1564,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239170656"/>
-        <c:axId val="239174576"/>
+        <c:axId val="374380912"/>
+        <c:axId val="374389144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239170656"/>
+        <c:axId val="374380912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,12 +1625,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239174576"/>
+        <c:crossAx val="374389144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239174576"/>
+        <c:axId val="374389144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1687,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239170656"/>
+        <c:crossAx val="374380912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1700,7 +1751,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1786,7 +1836,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1881,11 +1930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239174184"/>
-        <c:axId val="239171440"/>
+        <c:axId val="374380128"/>
+        <c:axId val="374382872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239174184"/>
+        <c:axId val="374380128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,12 +1991,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239171440"/>
+        <c:crossAx val="374382872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239171440"/>
+        <c:axId val="374382872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2004,7 +2053,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239174184"/>
+        <c:crossAx val="374380128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2068,7 +2117,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2154,7 +2202,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2249,11 +2296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239169480"/>
-        <c:axId val="239169088"/>
+        <c:axId val="374382480"/>
+        <c:axId val="374389536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239169480"/>
+        <c:axId val="374382480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2310,12 +2357,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239169088"/>
+        <c:crossAx val="374389536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239169088"/>
+        <c:axId val="374389536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2372,7 +2419,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239169480"/>
+        <c:crossAx val="374382480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2642,11 +2689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239174968"/>
-        <c:axId val="239172224"/>
+        <c:axId val="374380520"/>
+        <c:axId val="374382088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239174968"/>
+        <c:axId val="374380520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,12 +2750,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239172224"/>
+        <c:crossAx val="374382088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239172224"/>
+        <c:axId val="374382088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2765,7 +2812,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239174968"/>
+        <c:crossAx val="374380520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2998,11 +3045,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239173008"/>
-        <c:axId val="240602472"/>
+        <c:axId val="374381304"/>
+        <c:axId val="374389928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239173008"/>
+        <c:axId val="374381304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3059,12 +3106,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240602472"/>
+        <c:crossAx val="374389928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240602472"/>
+        <c:axId val="374389928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3121,7 +3168,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239173008"/>
+        <c:crossAx val="374381304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3399,11 +3446,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240603648"/>
-        <c:axId val="240607960"/>
+        <c:axId val="374390320"/>
+        <c:axId val="374383656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240603648"/>
+        <c:axId val="374390320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3460,12 +3507,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240607960"/>
+        <c:crossAx val="374383656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240607960"/>
+        <c:axId val="374383656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3522,7 +3569,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240603648"/>
+        <c:crossAx val="374390320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3611,7 +3658,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3697,7 +3743,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3792,11 +3837,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240604824"/>
-        <c:axId val="240607176"/>
+        <c:axId val="374381696"/>
+        <c:axId val="374385224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240604824"/>
+        <c:axId val="374381696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3853,12 +3898,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240607176"/>
+        <c:crossAx val="374385224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240607176"/>
+        <c:axId val="374385224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3915,7 +3960,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240604824"/>
+        <c:crossAx val="374381696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4004,7 +4049,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4140,11 +4184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240605216"/>
-        <c:axId val="240604040"/>
+        <c:axId val="374385616"/>
+        <c:axId val="374386008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240605216"/>
+        <c:axId val="374385616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4201,12 +4245,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240604040"/>
+        <c:crossAx val="374386008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240604040"/>
+        <c:axId val="374386008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4263,7 +4307,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240605216"/>
+        <c:crossAx val="374385616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4352,7 +4396,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4438,7 +4481,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4533,11 +4575,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240605608"/>
-        <c:axId val="240606000"/>
+        <c:axId val="374394240"/>
+        <c:axId val="374391496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240605608"/>
+        <c:axId val="374394240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4594,12 +4636,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240606000"/>
+        <c:crossAx val="374391496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240606000"/>
+        <c:axId val="374391496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4656,7 +4698,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240605608"/>
+        <c:crossAx val="374394240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4745,7 +4787,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5018,9 +5059,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5143,9 +5182,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5249,11 +5286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240600512"/>
-        <c:axId val="240603256"/>
+        <c:axId val="374393456"/>
+        <c:axId val="374393064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240600512"/>
+        <c:axId val="374393456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5310,12 +5347,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240603256"/>
+        <c:crossAx val="374393064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240603256"/>
+        <c:axId val="374393064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5372,7 +5409,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240600512"/>
+        <c:crossAx val="374393456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5437,7 +5474,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5523,7 +5559,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5618,11 +5653,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101417600"/>
-        <c:axId val="101414856"/>
+        <c:axId val="474868976"/>
+        <c:axId val="474874072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101417600"/>
+        <c:axId val="474868976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5679,12 +5714,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101414856"/>
+        <c:crossAx val="474874072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101414856"/>
+        <c:axId val="474874072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5741,7 +5776,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101417600"/>
+        <c:crossAx val="474868976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5830,7 +5865,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5966,11 +6000,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240601296"/>
-        <c:axId val="240601688"/>
+        <c:axId val="374391104"/>
+        <c:axId val="374391888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240601296"/>
+        <c:axId val="374391104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6027,12 +6061,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240601688"/>
+        <c:crossAx val="374391888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240601688"/>
+        <c:axId val="374391888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6089,7 +6123,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240601296"/>
+        <c:crossAx val="374391104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6178,7 +6212,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6364,11 +6397,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241096376"/>
-        <c:axId val="241099512"/>
+        <c:axId val="474874856"/>
+        <c:axId val="474870152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241096376"/>
+        <c:axId val="474874856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6425,12 +6458,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241099512"/>
+        <c:crossAx val="474870152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241099512"/>
+        <c:axId val="474870152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6487,7 +6520,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241096376"/>
+        <c:crossAx val="474874856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6576,7 +6609,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6762,11 +6794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241097552"/>
-        <c:axId val="241090888"/>
+        <c:axId val="474872112"/>
+        <c:axId val="474875248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241097552"/>
+        <c:axId val="474872112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6823,12 +6855,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241090888"/>
+        <c:crossAx val="474875248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241090888"/>
+        <c:axId val="474875248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6885,7 +6917,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241097552"/>
+        <c:crossAx val="474872112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6949,7 +6981,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7035,7 +7066,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -7130,11 +7160,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101413680"/>
-        <c:axId val="101414072"/>
+        <c:axId val="474863488"/>
+        <c:axId val="474869368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101413680"/>
+        <c:axId val="474863488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7191,12 +7221,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101414072"/>
+        <c:crossAx val="474869368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101414072"/>
+        <c:axId val="474869368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7253,7 +7283,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101413680"/>
+        <c:crossAx val="474863488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7317,7 +7347,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7403,7 +7432,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -7498,11 +7526,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101412504"/>
-        <c:axId val="101418384"/>
+        <c:axId val="474873288"/>
+        <c:axId val="474867800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101412504"/>
+        <c:axId val="474873288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7559,12 +7587,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101418384"/>
+        <c:crossAx val="474867800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101418384"/>
+        <c:axId val="474867800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7621,7 +7649,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101412504"/>
+        <c:crossAx val="474873288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7820,11 +7848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101412896"/>
-        <c:axId val="101415640"/>
+        <c:axId val="474873680"/>
+        <c:axId val="474872504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101412896"/>
+        <c:axId val="474873680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7881,12 +7909,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101415640"/>
+        <c:crossAx val="474872504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101415640"/>
+        <c:axId val="474872504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7943,7 +7971,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101412896"/>
+        <c:crossAx val="474873680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8186,11 +8214,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101414464"/>
-        <c:axId val="101419168"/>
+        <c:axId val="474870936"/>
+        <c:axId val="474863880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101414464"/>
+        <c:axId val="474870936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8247,12 +8275,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101419168"/>
+        <c:crossAx val="474863880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101419168"/>
+        <c:axId val="474863880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8309,7 +8337,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101414464"/>
+        <c:crossAx val="474870936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8373,7 +8401,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8459,7 +8486,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8554,11 +8580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101419560"/>
-        <c:axId val="101415248"/>
+        <c:axId val="474865056"/>
+        <c:axId val="374379344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101419560"/>
+        <c:axId val="474865056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8615,12 +8641,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101415248"/>
+        <c:crossAx val="374379344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101415248"/>
+        <c:axId val="374379344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8677,7 +8703,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101419560"/>
+        <c:crossAx val="474865056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8741,7 +8767,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8827,7 +8852,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8922,11 +8946,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239170264"/>
-        <c:axId val="239171048"/>
+        <c:axId val="374384440"/>
+        <c:axId val="374388360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239170264"/>
+        <c:axId val="374384440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8983,12 +9007,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239171048"/>
+        <c:crossAx val="374388360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239171048"/>
+        <c:axId val="374388360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9045,7 +9069,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239170264"/>
+        <c:crossAx val="374384440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9109,7 +9133,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9195,7 +9218,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -9290,11 +9312,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239175360"/>
-        <c:axId val="239169872"/>
+        <c:axId val="374386400"/>
+        <c:axId val="374386792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239175360"/>
+        <c:axId val="374386400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9351,12 +9373,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239169872"/>
+        <c:crossAx val="374386792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239169872"/>
+        <c:axId val="374386792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9413,7 +9435,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239175360"/>
+        <c:crossAx val="374386400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24078,8 +24100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -24352,6 +24374,770 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.25" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5"/>
+    <col min="4" max="4" width="16.25" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B2" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.91215999999999997</v>
+      </c>
+      <c r="D2" s="5">
+        <v>6.6183000000000006E-2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>6.0096999999999998E-2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4.1404000000000003E-2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3.3487999999999997E-2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>4.8550999999999997E-2</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2.5758E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B3" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.91415999999999997</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6.7070000000000005E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6.0659999999999999E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4.1716999999999997E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3.3779000000000003E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4.9119999999999997E-2</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2.6027999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B4" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.91603999999999997</v>
+      </c>
+      <c r="D4" s="5">
+        <v>6.7957000000000004E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6.1224000000000001E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4.2030999999999999E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3.4070999999999997E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>4.9688999999999997E-2</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2.6298999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B5" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.91780700000000004</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6.8844000000000002E-2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>6.1787000000000002E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4.2345000000000001E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3.4361999999999997E-2</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5.0257999999999997E-2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2.6568999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B6" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.91946700000000003</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6.9732000000000002E-2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.2350999999999997E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4.2658000000000001E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3.4653999999999997E-2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5.0826999999999997E-2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2.6838999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B7" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.92102700000000004</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7.0619000000000001E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6.2913999999999998E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4.2972000000000003E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>3.4944999999999997E-2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>5.1395999999999997E-2</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2.7109999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B8" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.92249300000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>7.1506E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>6.3478000000000007E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4.3284999999999997E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3.5236999999999997E-2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>5.1964999999999997E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2.7380000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B9" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.92386900000000005</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7.2392999999999999E-2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6.4041000000000001E-2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4.3598999999999999E-2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3.5527999999999997E-2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5.2534999999999998E-2</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2.7650000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.92516299999999996</v>
+      </c>
+      <c r="D10" s="5">
+        <v>7.3279999999999998E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>6.4604999999999996E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4.3913000000000001E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>3.5819999999999998E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>5.3103999999999998E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>2.7921000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>7.1895000000000001E-2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>7.1748999999999993E-2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.10800700000000001</v>
+      </c>
+      <c r="F14" s="5">
+        <v>7.0945999999999995E-2</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.109959</v>
+      </c>
+      <c r="H14" s="5">
+        <v>8.9993000000000004E-2</v>
+      </c>
+      <c r="I14" s="5">
+        <v>8.6415000000000006E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="5">
+        <v>3.3531999999999999E-2</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.105794</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.15306700000000001</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.101369</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.15270900000000001</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.12870999999999999</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0.119451</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3.2402E-2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.110552</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.15967600000000001</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.105832</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.159169</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.13433700000000001</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0.124554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3.1371000000000003E-2</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.11531</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.16628499999999999</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.110294</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.16563</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.139963</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0.12965699999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.7485000000000001E-2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.129332</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.18323600000000001</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.121847</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.180451</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.15445</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0.14160500000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.6399E-2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.134822</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.190662</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.12687000000000001</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.18757099999999999</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.160776</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0.14724899999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1.4054000000000001E-2</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.14166000000000001</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.19936899999999999</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.13308600000000001</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.19562499999999999</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.168292</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0.15382299999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.3094E-2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.147346</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.20699000000000001</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.13835</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.20286799999999999</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.174788</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0.15960299999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1.2257000000000001E-2</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.15296799999999999</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.21454300000000001</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.14349700000000001</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.21007799999999999</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.18123</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0.16533800000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.88592899999999997</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2.2707000000000001E-2</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1.8735000000000002E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1.2938E-2</v>
+      </c>
+      <c r="G26" s="5">
+        <v>8.8669999999999999E-3</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1.7905000000000001E-2</v>
+      </c>
+      <c r="I26" s="5">
+        <v>7.0260000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.885799</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2.3449999999999999E-2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1.9174E-2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="G27" s="5">
+        <v>9.0519999999999993E-3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1.8425E-2</v>
+      </c>
+      <c r="I27" s="5">
+        <v>7.1859999999999997E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.88555099999999998</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2.4192999999999999E-2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1.9612999999999998E-2</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1.3662000000000001E-2</v>
+      </c>
+      <c r="G28" s="5">
+        <v>9.2379999999999997E-3</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1.8945E-2</v>
+      </c>
+      <c r="I28" s="5">
+        <v>7.3460000000000001E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.88520600000000005</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2.4936E-2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>2.0052E-2</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1.4024E-2</v>
+      </c>
+      <c r="G29" s="5">
+        <v>9.4240000000000001E-3</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1.9465E-2</v>
+      </c>
+      <c r="I29" s="5">
+        <v>7.5059999999999997E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.88478400000000001</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2.5679E-2</v>
+      </c>
+      <c r="E30" s="5">
+        <v>2.0490999999999999E-2</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1.4385E-2</v>
+      </c>
+      <c r="G30" s="5">
+        <v>9.6100000000000005E-3</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1.9986E-2</v>
+      </c>
+      <c r="I30" s="5">
+        <v>7.6660000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0.884301</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2.6422000000000001E-2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>2.0929E-2</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1.4747E-2</v>
+      </c>
+      <c r="G31" s="5">
+        <v>9.7959999999999992E-3</v>
+      </c>
+      <c r="H31" s="5">
+        <v>2.0506E-2</v>
+      </c>
+      <c r="I31" s="5">
+        <v>7.8259999999999996E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0.883768</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2.7165000000000002E-2</v>
+      </c>
+      <c r="E32" s="5">
+        <v>2.1368000000000002E-2</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1.5108999999999999E-2</v>
+      </c>
+      <c r="G32" s="5">
+        <v>9.9819999999999996E-3</v>
+      </c>
+      <c r="H32" s="5">
+        <v>2.1026E-2</v>
+      </c>
+      <c r="I32" s="5">
+        <v>7.986E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0.88319700000000001</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2.7909E-2</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2.1807E-2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1.5469999999999999E-2</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1.0168E-2</v>
+      </c>
+      <c r="H33" s="5">
+        <v>2.1545999999999999E-2</v>
+      </c>
+      <c r="I33" s="5">
+        <v>8.1460000000000005E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0.88259600000000005</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2.8652E-2</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2.2245999999999998E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1.5831999999999999E-2</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1.0354E-2</v>
+      </c>
+      <c r="H34" s="5">
+        <v>2.2067E-2</v>
+      </c>
+      <c r="I34" s="5">
+        <v>8.3059999999999991E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
@@ -24625,7 +25411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>

</xml_diff>

<commit_message>
time to show result of fitting DT custom REE lib
</commit_message>
<xml_diff>
--- a/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
+++ b/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna (Repaired).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PosGeneral_SimGau" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
   <si>
     <t>Original Matching</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -309,6 +309,10 @@
   </si>
   <si>
     <t>band3(854-879)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABP-single</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1019,6 +1023,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1104,6 +1109,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1198,11 +1204,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474867016"/>
-        <c:axId val="474864664"/>
+        <c:axId val="357206840"/>
+        <c:axId val="357209976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474867016"/>
+        <c:axId val="357206840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,12 +1265,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474864664"/>
+        <c:crossAx val="357209976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474864664"/>
+        <c:axId val="357209976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1327,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474867016"/>
+        <c:crossAx val="357206840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1385,6 +1391,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1425,17 +1432,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PosGeneral_SimCorrcoef!$G$2</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Band3</c:v>
+                  <c:v>Band2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1470,6 +1477,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1502,6 +1510,33 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>PosGeneral_SimCorrcoef!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.5871000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5073E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1730000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.9581999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0244000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.1901999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>PosGeneral_SimCorrcoef!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
@@ -1523,33 +1558,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.3759999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>PosGeneral_SimCorrcoef!$G$3:$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.7984999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.8571000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5800999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.58E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.9873999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.7720000000000003E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1564,16 +1572,78 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374380912"/>
-        <c:axId val="374389144"/>
+        <c:axId val="358098248"/>
+        <c:axId val="358094720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374380912"/>
+        <c:axId val="358098248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358094720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="358094720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1625,69 +1695,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374389144"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="374389144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="374380912"/>
+        <c:crossAx val="358098248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1751,6 +1759,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1791,11 +1800,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PosGeneral_SimCorrcoef!$H$2</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG_Band</c:v>
+                  <c:v>Band3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1836,6 +1845,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1895,27 +1905,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PosGeneral_SimCorrcoef!$H$3:$H$8</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.8169666666666664E-2</c:v>
+                  <c:v>2.7984999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9161000000000001E-2</c:v>
+                  <c:v>1.8571000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4725333333333333E-2</c:v>
+                  <c:v>1.5800999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1473333333333335E-3</c:v>
+                  <c:v>9.58E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1752000000000004E-2</c:v>
+                  <c:v>1.9873999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.146333333333333E-3</c:v>
+                  <c:v>7.7720000000000003E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1930,11 +1940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374380128"/>
-        <c:axId val="374382872"/>
+        <c:axId val="358097072"/>
+        <c:axId val="358097464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374380128"/>
+        <c:axId val="358097072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,12 +2001,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374382872"/>
+        <c:crossAx val="358097464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374382872"/>
+        <c:axId val="358097464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2063,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374380128"/>
+        <c:crossAx val="358097072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2117,6 +2127,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2157,11 +2168,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PosGeneral_SimCorrcoef!$I$2</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.5,0.3,0.2</c:v>
+                  <c:v>AVG_Band</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2202,6 +2213,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2261,27 +2273,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PosGeneral_SimCorrcoef!$I$3:$I$8</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$H$3:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.9684799999999999E-2</c:v>
+                  <c:v>3.8169666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0155599999999999E-2</c:v>
+                  <c:v>1.9161000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.55131E-2</c:v>
+                  <c:v>1.4725333333333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7634000000000001E-3</c:v>
+                  <c:v>1.1473333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2617000000000002E-2</c:v>
+                  <c:v>2.1752000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7682999999999996E-3</c:v>
+                  <c:v>3.146333333333333E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2296,11 +2308,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374382480"/>
-        <c:axId val="374389536"/>
+        <c:axId val="358095896"/>
+        <c:axId val="358099032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374382480"/>
+        <c:axId val="358095896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2357,12 +2369,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374389536"/>
+        <c:crossAx val="358099032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374389536"/>
+        <c:axId val="358099032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,7 +2431,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374382480"/>
+        <c:crossAx val="358095896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2469,6 +2481,374 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PosGeneral_SimCorrcoef!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.5,0.3,0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PosGeneral_SimCorrcoef!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PosGeneral_SimCorrcoef!$I$3:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.9684799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0155599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.55131E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7634000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2617000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7682999999999996E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="358096288"/>
+        <c:axId val="358093544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="358096288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358093544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="358093544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358096288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2689,11 +3069,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374380520"/>
-        <c:axId val="374382088"/>
+        <c:axId val="357207232"/>
+        <c:axId val="357208016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374380520"/>
+        <c:axId val="357207232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,12 +3130,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374382088"/>
+        <c:crossAx val="357208016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374382088"/>
+        <c:axId val="357208016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2812,7 +3192,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374380520"/>
+        <c:crossAx val="357207232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2861,7 +3241,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3045,11 +3425,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374381304"/>
-        <c:axId val="374389928"/>
+        <c:axId val="357205272"/>
+        <c:axId val="358038592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374381304"/>
+        <c:axId val="357205272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3106,12 +3486,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374389928"/>
+        <c:crossAx val="358038592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374389928"/>
+        <c:axId val="358038592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,408 +3548,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374381304"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Band3-</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Amount</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Possibility!$J$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Amount</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Possibility!$D$3:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3.4022999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4216999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0281E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2799E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5295999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0333999999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Possibility!$J$3:$J$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.8330000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4220000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6160000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.175</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8660000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3759999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="374390320"/>
-        <c:axId val="374383656"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="374390320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="374383656"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="374383656"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="374390320"/>
+        <c:crossAx val="357205272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3653,7 +3632,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Band1</a:t>
+              <a:t>Band3-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Amount</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3698,7 +3685,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PosGen_SimFrechet!$J$2</c:f>
+              <c:f>Possibility!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3775,34 +3762,34 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>PosGen_SimFrechet!$B$3:$B$8</c:f>
+              <c:f>Possibility!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.3730000000000004E-2</c:v>
+                  <c:v>3.4022999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1232000000000002E-2</c:v>
+                  <c:v>2.4216999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6077E-2</c:v>
+                  <c:v>2.0281E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6794E-2</c:v>
+                  <c:v>1.2799E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1180999999999997E-2</c:v>
+                  <c:v>2.5295999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9152999999999998E-2</c:v>
+                  <c:v>1.0333999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PosGen_SimFrechet!$J$3:$J$8</c:f>
+              <c:f>Possibility!$J$3:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3837,11 +3824,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374381696"/>
-        <c:axId val="374385224"/>
+        <c:axId val="358042904"/>
+        <c:axId val="358040552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374381696"/>
+        <c:axId val="358042904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3898,12 +3885,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374385224"/>
+        <c:crossAx val="358040552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374385224"/>
+        <c:axId val="358040552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3960,7 +3947,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374381696"/>
+        <c:crossAx val="358042904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4044,11 +4031,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Band2</a:t>
+              <a:t>Band1</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4120,29 +4108,74 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>PosGen_SimFrechet!$C$3:$C$8</c:f>
+              <c:f>PosGen_SimFrechet!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.106961</c:v>
+                  <c:v>7.3730000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14255999999999999</c:v>
+                  <c:v>6.1232000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.101796</c:v>
+                  <c:v>4.6077E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17202100000000001</c:v>
+                  <c:v>3.6794E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.128048</c:v>
+                  <c:v>5.1180999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12737899999999999</c:v>
+                  <c:v>2.9152999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4184,11 +4217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374385616"/>
-        <c:axId val="374386008"/>
+        <c:axId val="358038984"/>
+        <c:axId val="358039376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374385616"/>
+        <c:axId val="358038984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4245,12 +4278,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374386008"/>
+        <c:crossAx val="358039376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374386008"/>
+        <c:axId val="358039376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4307,7 +4340,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374385616"/>
+        <c:crossAx val="358038984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4391,11 +4424,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Band3</a:t>
+              <a:t>Band2</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4467,73 +4501,29 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>PosGen_SimFrechet!$D$3:$D$8</c:f>
+              <c:f>PosGen_SimFrechet!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.8923000000000001E-2</c:v>
+                  <c:v>0.106961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0711E-2</c:v>
+                  <c:v>0.14255999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6929E-2</c:v>
+                  <c:v>0.101796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0801E-2</c:v>
+                  <c:v>0.17202100000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.162E-2</c:v>
+                  <c:v>0.128048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.7139999999999995E-3</c:v>
+                  <c:v>0.12737899999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4575,11 +4565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374394240"/>
-        <c:axId val="374391496"/>
+        <c:axId val="358041336"/>
+        <c:axId val="358041728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374394240"/>
+        <c:axId val="358041336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4636,12 +4626,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374391496"/>
+        <c:crossAx val="358041728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374391496"/>
+        <c:axId val="358041728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4698,7 +4688,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374394240"/>
+        <c:crossAx val="358041336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4782,11 +4772,771 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Band3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PosGen_SimFrechet!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8923000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0711E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6929E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0801E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.162E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7139999999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="358035456"/>
+        <c:axId val="358037808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="358035456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358037808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="358037808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="358035456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PosGeneral_SimGau!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Band2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PosGeneral_SimGau!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PosGeneral_SimGau!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.108625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15229000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14880299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.128418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.116984</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="357211152"/>
+        <c:axId val="357211544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="357211152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="357211544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="357211544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="357211152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
               <a:t>band1</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5059,7 +5809,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5182,7 +5934,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5286,11 +6040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374393456"/>
-        <c:axId val="374393064"/>
+        <c:axId val="358037416"/>
+        <c:axId val="358035848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374393456"/>
+        <c:axId val="358037416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5347,12 +6101,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374393064"/>
+        <c:crossAx val="358035848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374393064"/>
+        <c:axId val="358035848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5409,7 +6163,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374393456"/>
+        <c:crossAx val="358037416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5459,373 +6213,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>PosGeneral_SimGau!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Band2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>PosGeneral_SimGau!$B$3:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.8330000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4220000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6160000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.175</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8660000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3759999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>PosGeneral_SimGau!$F$3:$F$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.108625</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.15229000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.10147</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.14880299999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.128418</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.116984</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="474868976"/>
-        <c:axId val="474874072"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="474868976"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="474874072"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="474874072"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="474868976"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5865,6 +6253,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6000,11 +6389,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374391104"/>
-        <c:axId val="374391888"/>
+        <c:axId val="358036632"/>
+        <c:axId val="358037024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374391104"/>
+        <c:axId val="358036632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6061,12 +6450,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374391888"/>
+        <c:crossAx val="358037024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374391888"/>
+        <c:axId val="358037024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6123,7 +6512,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374391104"/>
+        <c:crossAx val="358036632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6172,7 +6561,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6212,6 +6601,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6397,11 +6787,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474874856"/>
-        <c:axId val="474870152"/>
+        <c:axId val="359201088"/>
+        <c:axId val="359201480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474874856"/>
+        <c:axId val="359201088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6458,12 +6848,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474870152"/>
+        <c:crossAx val="359201480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474870152"/>
+        <c:axId val="359201480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6520,7 +6910,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474874856"/>
+        <c:crossAx val="359201088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6569,7 +6959,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6609,6 +6999,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6794,11 +7185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474872112"/>
-        <c:axId val="474875248"/>
+        <c:axId val="359205008"/>
+        <c:axId val="359204224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474872112"/>
+        <c:axId val="359205008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6855,12 +7246,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474875248"/>
+        <c:crossAx val="359204224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474875248"/>
+        <c:axId val="359204224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6917,7 +7308,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474872112"/>
+        <c:crossAx val="359205008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6981,6 +7372,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7066,6 +7458,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -7160,11 +7553,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474863488"/>
-        <c:axId val="474869368"/>
+        <c:axId val="357208800"/>
+        <c:axId val="357209584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474863488"/>
+        <c:axId val="357208800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7221,12 +7614,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474869368"/>
+        <c:crossAx val="357209584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474869368"/>
+        <c:axId val="357209584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7283,7 +7676,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474863488"/>
+        <c:crossAx val="357208800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7526,11 +7919,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474873288"/>
-        <c:axId val="474867800"/>
+        <c:axId val="357207624"/>
+        <c:axId val="357204096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474873288"/>
+        <c:axId val="357207624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7587,12 +7980,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474867800"/>
+        <c:crossAx val="357204096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474867800"/>
+        <c:axId val="357204096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7649,7 +8042,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474873288"/>
+        <c:crossAx val="357207624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7848,11 +8241,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474873680"/>
-        <c:axId val="474872504"/>
+        <c:axId val="357210368"/>
+        <c:axId val="357209192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474873680"/>
+        <c:axId val="357210368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7909,12 +8302,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474872504"/>
+        <c:crossAx val="357209192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474872504"/>
+        <c:axId val="357209192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7971,7 +8364,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474873680"/>
+        <c:crossAx val="357210368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8214,11 +8607,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474870936"/>
-        <c:axId val="474863880"/>
+        <c:axId val="358094328"/>
+        <c:axId val="358099424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474870936"/>
+        <c:axId val="358094328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8275,12 +8668,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474863880"/>
+        <c:crossAx val="358099424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="474863880"/>
+        <c:axId val="358099424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8337,7 +8730,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474870936"/>
+        <c:crossAx val="358094328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8401,6 +8794,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8486,6 +8880,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -8580,11 +8975,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="474865056"/>
-        <c:axId val="374379344"/>
+        <c:axId val="358095112"/>
+        <c:axId val="358096680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="474865056"/>
+        <c:axId val="358095112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8641,12 +9036,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374379344"/>
+        <c:crossAx val="358096680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374379344"/>
+        <c:axId val="358096680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8703,7 +9098,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474865056"/>
+        <c:crossAx val="358095112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8767,6 +9162,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8807,17 +9203,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PosGeneral_SimCorrcoef!$E$2</c:f>
+              <c:f>'Band2-90%'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Band1</c:v>
+                  <c:v>ABP-single</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -8838,100 +9234,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="zh-CN"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>PosGeneral_SimCorrcoef!$E$3:$E$8</c:f>
+              <c:f>'Band2-90%'!$B$3:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.0653000000000002E-2</c:v>
+                  <c:v>2.8330000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3838999999999999E-2</c:v>
+                  <c:v>2.4220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9202E-2</c:v>
+                  <c:v>1.6160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3443999999999999E-2</c:v>
+                  <c:v>1.175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5138000000000001E-2</c:v>
+                  <c:v>1.8660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3568999999999999E-2</c:v>
+                  <c:v>1.3759999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PosGeneral_SimCorrcoef!$B$3:$B$8</c:f>
+              <c:f>'Band2-90%'!$F$3:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.8330000000000002</c:v>
+                  <c:v>0.10997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4220000000000002</c:v>
+                  <c:v>0.154443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6160000000000001</c:v>
+                  <c:v>0.102285</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.175</c:v>
+                  <c:v>0.14943200000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8660000000000001</c:v>
+                  <c:v>0.12986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3759999999999999</c:v>
+                  <c:v>0.117855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8946,16 +9298,78 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374384440"/>
-        <c:axId val="374388360"/>
+        <c:axId val="361229288"/>
+        <c:axId val="361230464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374384440"/>
+        <c:axId val="361229288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361230464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="361230464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -9007,69 +9421,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374388360"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="374388360"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="374384440"/>
+        <c:crossAx val="361229288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9133,6 +9485,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9173,11 +9526,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PosGeneral_SimCorrcoef!$F$2</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Band2</c:v>
+                  <c:v>Band1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9218,6 +9571,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -9250,27 +9604,27 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>PosGeneral_SimCorrcoef!$F$3:$F$8</c:f>
+              <c:f>PosGeneral_SimCorrcoef!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.5871000000000002E-2</c:v>
+                  <c:v>4.0653000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5073E-2</c:v>
+                  <c:v>2.3838999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1730000000000006E-3</c:v>
+                  <c:v>1.9202E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.9581999999999999E-2</c:v>
+                  <c:v>1.3443999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0244000000000002E-2</c:v>
+                  <c:v>2.5138000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1901999999999999E-2</c:v>
+                  <c:v>1.3568999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9312,11 +9666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374386400"/>
-        <c:axId val="374386792"/>
+        <c:axId val="358092760"/>
+        <c:axId val="358093936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374386400"/>
+        <c:axId val="358092760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9373,12 +9727,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374386792"/>
+        <c:crossAx val="358093936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374386792"/>
+        <c:axId val="358093936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9435,7 +9789,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374386400"/>
+        <c:crossAx val="358092760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10084,6 +10438,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -18104,6 +18498,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -21928,6 +22838,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -23547,8 +24487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23582,7 +24522,9 @@
       <c r="E2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
         <v>57</v>
@@ -23611,7 +24553,9 @@
         <f>C3*D3</f>
         <v>5578.080465</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5">
+        <v>0.10997</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="12">
         <v>9.7620000000000005</v>
@@ -23640,7 +24584,9 @@
         <f t="shared" ref="E4:E8" si="0">C4*D4</f>
         <v>16395.897371999999</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>0.154443</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="13">
         <v>8.6479999999999997</v>
@@ -23669,7 +24615,9 @@
         <f t="shared" si="0"/>
         <v>1922.9825309999999</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5">
+        <v>0.102285</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="13">
         <v>5.516</v>
@@ -23698,7 +24646,9 @@
         <f t="shared" si="0"/>
         <v>16507.130925000001</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>0.14943200000000001</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="13">
         <v>4.2450000000000001</v>
@@ -23727,7 +24677,9 @@
         <f t="shared" si="0"/>
         <v>9317.6863200000007</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>0.12986</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="13">
         <v>6.68</v>
@@ -23756,7 +24708,9 @@
         <f t="shared" si="0"/>
         <v>10456.615777999999</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>0.117855</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="13">
         <v>4.5990000000000002</v>
@@ -24377,7 +25331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>